<commit_message>
Added datasets to the tutorial package, updated tutorial to run from the R package
</commit_message>
<xml_diff>
--- a/Tutorial/EncountersDistanceTutorial.xlsx
+++ b/Tutorial/EncountersDistanceTutorial.xlsx
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="8">
-  <si>
-    <t xml:space="preserve">Lake name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="6">
   <si>
     <t xml:space="preserve">Observer name</t>
   </si>
@@ -35,9 +32,6 @@
   </si>
   <si>
     <t xml:space="preserve">size</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lake Burgan</t>
   </si>
   <si>
     <t xml:space="preserve">Aislyn</t>
@@ -151,7 +145,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1048576"/>
+  <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
@@ -161,9 +155,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="1" style="0" width="21.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1016" min="12" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1017" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="1" style="0" width="21.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1015" min="11" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1016" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -179,415 +173,340 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>64</v>
-      </c>
-      <c r="E2" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>1</v>
+        <v>38</v>
       </c>
       <c r="D3" s="1" t="n">
-        <v>38</v>
-      </c>
-      <c r="E3" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="D4" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="E4" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>2</v>
+        <v>38</v>
       </c>
       <c r="D5" s="1" t="n">
-        <v>38</v>
-      </c>
-      <c r="E5" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="D6" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="E6" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="D7" s="1" t="n">
-        <v>19</v>
-      </c>
-      <c r="E7" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D9" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="E9" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="D10" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="E10" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="D11" s="1" t="n">
-        <v>39</v>
-      </c>
-      <c r="E11" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D12" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="E12" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1" t="n">
         <v>6</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>6</v>
+        <v>55</v>
       </c>
       <c r="D13" s="1" t="n">
-        <v>55</v>
-      </c>
-      <c r="E13" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1" t="n">
         <v>6</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D14" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="E14" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1" t="n">
         <v>6</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="D15" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="E15" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1" t="n">
         <v>6</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D16" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="E16" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>7</v>
+        <v>68</v>
       </c>
       <c r="D17" s="1" t="n">
-        <v>68</v>
-      </c>
-      <c r="E17" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B18" s="1" t="n">
+        <v>8</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D18" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="E18" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>8</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>56</v>
-      </c>
-      <c r="E19" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B20" s="1" t="n">
+        <v>9</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>9.5</v>
-      </c>
-      <c r="E20" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B21" s="1" t="n">
+        <v>9</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D21" s="1" t="n">
-        <v>20</v>
-      </c>
-      <c r="E21" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B22" s="1" t="n">
+        <v>9</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="D22" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="E22" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>9</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D23" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E23" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B24" s="1" t="n">
+        <v>10</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="D24" s="1" t="n">
-        <v>42</v>
-      </c>
-      <c r="E24" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B25" s="1" t="n">
+        <v>10</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="D25" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="E25" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -595,16 +514,13 @@
       <c r="A26" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>7</v>
+      <c r="B26" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="C26" s="1" t="n">
-        <v>1</v>
+        <v>48</v>
       </c>
       <c r="D26" s="1" t="n">
-        <v>48</v>
-      </c>
-      <c r="E26" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -612,16 +528,13 @@
       <c r="A27" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>7</v>
+      <c r="B27" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="C27" s="1" t="n">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="D27" s="1" t="n">
-        <v>32</v>
-      </c>
-      <c r="E27" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -629,16 +542,13 @@
       <c r="A28" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>7</v>
+      <c r="B28" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D28" s="1" t="n">
-        <v>21</v>
-      </c>
-      <c r="E28" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -646,16 +556,13 @@
       <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>7</v>
+      <c r="B29" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D29" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="E29" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -663,16 +570,13 @@
       <c r="A30" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>7</v>
+      <c r="B30" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="D30" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="E30" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -680,16 +584,13 @@
       <c r="A31" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>7</v>
+      <c r="B31" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D31" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="E31" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -697,16 +598,13 @@
       <c r="A32" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>7</v>
+      <c r="B32" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="D32" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="E32" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -714,16 +612,13 @@
       <c r="A33" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>7</v>
+      <c r="B33" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="D33" s="1" t="n">
-        <v>37</v>
-      </c>
-      <c r="E33" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -731,16 +626,13 @@
       <c r="A34" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>7</v>
+      <c r="B34" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="D34" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="E34" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -748,16 +640,13 @@
       <c r="A35" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>7</v>
+      <c r="B35" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="D35" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="E35" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -765,16 +654,13 @@
       <c r="A36" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>7</v>
+      <c r="B36" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E36" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -782,16 +668,13 @@
       <c r="A37" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>7</v>
+      <c r="B37" s="1" t="n">
+        <v>8</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D37" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E37" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -799,16 +682,13 @@
       <c r="A38" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>7</v>
+      <c r="B38" s="1" t="n">
+        <v>9</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>23</v>
-      </c>
-      <c r="E38" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -816,16 +696,13 @@
       <c r="A39" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>7</v>
+      <c r="B39" s="1" t="n">
+        <v>9</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D39" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="E39" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -833,16 +710,13 @@
       <c r="A40" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>7</v>
+      <c r="B40" s="1" t="n">
+        <v>9</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>50</v>
-      </c>
-      <c r="E40" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -850,16 +724,13 @@
       <c r="A41" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>7</v>
+      <c r="B41" s="1" t="n">
+        <v>9</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="D41" s="1" t="n">
-        <v>38</v>
-      </c>
-      <c r="E41" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -867,16 +738,13 @@
       <c r="A42" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>7</v>
+      <c r="B42" s="1" t="n">
+        <v>9</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="D42" s="1" t="n">
-        <v>26</v>
-      </c>
-      <c r="E42" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -884,16 +752,13 @@
       <c r="A43" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>7</v>
+      <c r="B43" s="1" t="n">
+        <v>9</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="D43" s="1" t="n">
-        <v>40</v>
-      </c>
-      <c r="E43" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -901,16 +766,13 @@
       <c r="A44" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>7</v>
+      <c r="B44" s="1" t="n">
+        <v>9</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D44" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="E44" s="1" t="n">
         <v>3</v>
       </c>
     </row>
@@ -918,16 +780,13 @@
       <c r="A45" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>7</v>
+      <c r="B45" s="1" t="n">
+        <v>9</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="D45" s="1" t="n">
-        <v>36</v>
-      </c>
-      <c r="E45" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -935,271 +794,223 @@
       <c r="A46" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>7</v>
+      <c r="B46" s="1" t="n">
+        <v>10</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="D46" s="1" t="n">
-        <v>67</v>
-      </c>
-      <c r="E46" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B47" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D47" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="E47" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B48" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="D48" s="1" t="n">
-        <v>30</v>
-      </c>
-      <c r="E48" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B49" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>11</v>
+        <v>64</v>
       </c>
       <c r="D49" s="1" t="n">
-        <v>64</v>
-      </c>
-      <c r="E49" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B50" s="1" t="n">
+        <v>12</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D50" s="1" t="n">
-        <v>34</v>
-      </c>
-      <c r="E50" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B51" s="1" t="n">
+        <v>12</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D51" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="E51" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B52" s="1" t="n">
+        <v>13</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="D52" s="1" t="n">
-        <v>33</v>
-      </c>
-      <c r="E52" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B53" s="1" t="n">
+        <v>14</v>
       </c>
       <c r="C53" s="1" t="n">
         <v>14</v>
       </c>
       <c r="D53" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="E53" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B54" s="1" t="n">
+        <v>14</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="D54" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="E54" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B55" s="1" t="n">
+        <v>14</v>
       </c>
       <c r="C55" s="1" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D55" s="1" t="n">
-        <v>16</v>
-      </c>
-      <c r="E55" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B56" s="1" t="n">
+        <v>14</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D56" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="E56" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B57" s="1" t="n">
+        <v>14</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D57" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="E57" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B58" s="1" t="n">
+        <v>14</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="D58" s="1" t="n">
-        <v>58</v>
-      </c>
-      <c r="E58" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B59" s="1" t="n">
+        <v>14</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="D59" s="1" t="n">
-        <v>69</v>
-      </c>
-      <c r="E59" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B60" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="D60" s="1" t="n">
-        <v>54</v>
-      </c>
-      <c r="E60" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="B61" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D61" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="E61" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1207,16 +1018,13 @@
       <c r="A62" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>7</v>
+      <c r="B62" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="D62" s="1" t="n">
-        <v>31</v>
-      </c>
-      <c r="E62" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1224,16 +1032,13 @@
       <c r="A63" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>7</v>
+      <c r="B63" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="D63" s="1" t="n">
-        <v>82</v>
-      </c>
-      <c r="E63" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1241,16 +1046,13 @@
       <c r="A64" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>7</v>
+      <c r="B64" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="C64" s="1" t="n">
-        <v>11</v>
+        <v>60</v>
       </c>
       <c r="D64" s="1" t="n">
-        <v>60</v>
-      </c>
-      <c r="E64" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1258,16 +1060,13 @@
       <c r="A65" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B65" s="1" t="s">
-        <v>7</v>
+      <c r="B65" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="C65" s="1" t="n">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="D65" s="1" t="n">
-        <v>45</v>
-      </c>
-      <c r="E65" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1275,16 +1074,13 @@
       <c r="A66" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B66" s="1" t="s">
-        <v>7</v>
+      <c r="B66" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="D66" s="1" t="n">
-        <v>54</v>
-      </c>
-      <c r="E66" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1292,16 +1088,13 @@
       <c r="A67" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B67" s="1" t="s">
-        <v>7</v>
+      <c r="B67" s="1" t="n">
+        <v>13</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="D67" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="E67" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1309,16 +1102,13 @@
       <c r="A68" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>7</v>
+      <c r="B68" s="1" t="n">
+        <v>13</v>
       </c>
       <c r="C68" s="1" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D68" s="1" t="n">
-        <v>12</v>
-      </c>
-      <c r="E68" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1326,16 +1116,13 @@
       <c r="A69" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B69" s="1" t="s">
-        <v>7</v>
+      <c r="B69" s="1" t="n">
+        <v>13</v>
       </c>
       <c r="C69" s="1" t="n">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="D69" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="E69" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1343,16 +1130,13 @@
       <c r="A70" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B70" s="1" t="s">
-        <v>7</v>
+      <c r="B70" s="1" t="n">
+        <v>14</v>
       </c>
       <c r="C70" s="1" t="n">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="D70" s="1" t="n">
-        <v>90</v>
-      </c>
-      <c r="E70" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1360,16 +1144,13 @@
       <c r="A71" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B71" s="1" t="s">
-        <v>7</v>
+      <c r="B71" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="C71" s="1" t="n">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="D71" s="1" t="n">
-        <v>41</v>
-      </c>
-      <c r="E71" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1377,16 +1158,13 @@
       <c r="A72" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B72" s="1" t="s">
-        <v>7</v>
+      <c r="B72" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="C72" s="1" t="n">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="D72" s="1" t="n">
-        <v>55</v>
-      </c>
-      <c r="E72" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1394,16 +1172,13 @@
       <c r="A73" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B73" s="1" t="s">
-        <v>7</v>
+      <c r="B73" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="C73" s="1" t="n">
-        <v>15</v>
+        <v>98</v>
       </c>
       <c r="D73" s="1" t="n">
-        <v>98</v>
-      </c>
-      <c r="E73" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1411,16 +1186,13 @@
       <c r="A74" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B74" s="1" t="s">
-        <v>7</v>
+      <c r="B74" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="C74" s="1" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D74" s="1" t="n">
-        <v>13</v>
-      </c>
-      <c r="E74" s="1" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1428,16 +1200,13 @@
       <c r="A75" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B75" s="1" t="s">
-        <v>7</v>
+      <c r="B75" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D75" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="E75" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1445,16 +1214,13 @@
       <c r="A76" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B76" s="1" t="s">
-        <v>7</v>
+      <c r="B76" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="C76" s="1" t="n">
         <v>15</v>
       </c>
       <c r="D76" s="1" t="n">
-        <v>15</v>
-      </c>
-      <c r="E76" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1462,16 +1228,13 @@
       <c r="A77" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B77" s="1" t="s">
-        <v>7</v>
+      <c r="B77" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="C77" s="1" t="n">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D77" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="E77" s="1" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1479,16 +1242,13 @@
       <c r="A78" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B78" s="1" t="s">
-        <v>7</v>
+      <c r="B78" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="C78" s="1" t="n">
-        <v>15</v>
+        <v>93</v>
       </c>
       <c r="D78" s="1" t="n">
-        <v>93</v>
-      </c>
-      <c r="E78" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1496,16 +1256,13 @@
       <c r="A79" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>7</v>
+      <c r="B79" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="C79" s="1" t="n">
-        <v>15</v>
+        <v>85</v>
       </c>
       <c r="D79" s="1" t="n">
-        <v>85</v>
-      </c>
-      <c r="E79" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1513,16 +1270,13 @@
       <c r="A80" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B80" s="1" t="s">
-        <v>7</v>
+      <c r="B80" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="C80" s="1" t="n">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="D80" s="1" t="n">
-        <v>25</v>
-      </c>
-      <c r="E80" s="1" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>